<commit_message>
Added unicode header support
Input csv can be ascii or unicode.
</commit_message>
<xml_diff>
--- a/workflow_testing.xlsx
+++ b/workflow_testing.xlsx
@@ -536,46 +536,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
@@ -592,6 +559,40 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -601,7 +602,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,7 +874,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -894,51 +894,51 @@
     <col min="8" max="9" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.6640625" customWidth="1"/>
-    <col min="17" max="18" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="34" t="s">
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="35"/>
-      <c r="K1" s="32" t="s">
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="55"/>
+      <c r="K1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" s="33" t="s">
+      <c r="L1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="P1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="R1" s="33" t="s">
-        <v>2</v>
-      </c>
-      <c r="S1" s="34" t="s">
+      <c r="Q1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="S1" s="27" t="s">
         <v>3</v>
       </c>
     </row>
@@ -955,16 +955,16 @@
       <c r="D2" s="14">
         <v>42009</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="33" t="s">
+      <c r="G2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="27" t="s">
         <v>29</v>
       </c>
       <c r="K2" s="11">
@@ -1046,7 +1046,7 @@
       <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="13">
@@ -1096,7 +1096,7 @@
       <c r="A5" s="11">
         <v>1</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="13">
@@ -1246,7 +1246,7 @@
       <c r="A8" s="11">
         <v>2</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="13">
@@ -1288,7 +1288,7 @@
       <c r="A9" s="11">
         <v>2</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="B9" s="48" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="13">
@@ -1297,13 +1297,13 @@
       <c r="D9" s="14">
         <v>42044</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
       <c r="K9" s="11"/>
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
@@ -1325,7 +1325,7 @@
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="44" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="13">
@@ -1334,16 +1334,16 @@
       <c r="D10" s="14">
         <v>42049</v>
       </c>
-      <c r="F10" s="32" t="s">
+      <c r="F10" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="33" t="s">
+      <c r="G10" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="27" t="s">
         <v>28</v>
       </c>
       <c r="K10" s="11"/>
@@ -1392,12 +1392,12 @@
       <c r="L11" s="12"/>
       <c r="M11" s="16"/>
       <c r="N11" s="17"/>
-      <c r="P11" s="31" t="s">
+      <c r="P11" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="Q11" s="31"/>
-      <c r="R11" s="31"/>
-      <c r="S11" s="31"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="59"/>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="11"/>
@@ -1422,12 +1422,12 @@
       <c r="N12" s="19"/>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="29"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
       <c r="F13" s="11">
         <v>1</v>
       </c>
@@ -1440,20 +1440,20 @@
       <c r="I13" s="14">
         <v>42024</v>
       </c>
-      <c r="K13" s="27" t="s">
+      <c r="K13" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="29"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="51"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
       <c r="F14" s="11">
         <v>2</v>
       </c>
@@ -1466,12 +1466,12 @@
       <c r="I14" s="14">
         <v>42034</v>
       </c>
-      <c r="K14" s="30" t="s">
+      <c r="K14" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
     </row>
     <row r="15" spans="1:19">
       <c r="F15" s="11">
@@ -1507,210 +1507,210 @@
     </row>
     <row r="17" spans="1:20" ht="15" thickBot="1"/>
     <row r="18" spans="1:20">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="42"/>
-      <c r="J18" s="59" t="s">
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="58"/>
+      <c r="J18" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="60"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
-      <c r="N18" s="61"/>
-      <c r="P18" s="40" t="s">
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="62"/>
+      <c r="P18" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="41"/>
-      <c r="T18" s="42"/>
+      <c r="Q18" s="57"/>
+      <c r="R18" s="57"/>
+      <c r="S18" s="57"/>
+      <c r="T18" s="58"/>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="43"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="44"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="53"/>
-      <c r="P19" s="54"/>
-      <c r="Q19" s="52"/>
-      <c r="R19" s="36"/>
-      <c r="S19" s="36"/>
-      <c r="T19" s="44"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="33"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="30"/>
+      <c r="L19" s="30"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="42"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="28"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="33"/>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="45"/>
+      <c r="A20" s="34"/>
       <c r="B20" s="5"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="44"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="36"/>
-      <c r="L20" s="36"/>
-      <c r="M20" s="36"/>
-      <c r="N20" s="44"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="36"/>
-      <c r="R20" s="36"/>
-      <c r="S20" s="36"/>
-      <c r="T20" s="44"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="33"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="33"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
+      <c r="S20" s="28"/>
+      <c r="T20" s="33"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="46"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="12"/>
       <c r="C21" s="6"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="47"/>
-      <c r="J21" s="46"/>
+      <c r="E21" s="36"/>
+      <c r="J21" s="35"/>
       <c r="K21" s="12"/>
       <c r="L21" s="6"/>
       <c r="M21" s="12"/>
-      <c r="N21" s="47"/>
-      <c r="P21" s="46"/>
+      <c r="N21" s="36"/>
+      <c r="P21" s="35"/>
       <c r="Q21" s="12"/>
       <c r="R21" s="6"/>
       <c r="S21" s="12"/>
-      <c r="T21" s="47"/>
+      <c r="T21" s="36"/>
     </row>
     <row r="22" spans="1:20">
-      <c r="A22" s="46"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="47"/>
-      <c r="J22" s="46"/>
+      <c r="E22" s="36"/>
+      <c r="J22" s="35"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="47"/>
-      <c r="P22" s="46"/>
+      <c r="N22" s="36"/>
+      <c r="P22" s="35"/>
       <c r="Q22" s="12"/>
       <c r="R22" s="12"/>
       <c r="S22" s="7"/>
-      <c r="T22" s="47"/>
+      <c r="T22" s="36"/>
     </row>
     <row r="23" spans="1:20">
-      <c r="A23" s="46"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
-      <c r="E23" s="48"/>
-      <c r="J23" s="46"/>
+      <c r="E23" s="37"/>
+      <c r="J23" s="35"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
-      <c r="N23" s="44"/>
-      <c r="P23" s="46"/>
+      <c r="N23" s="33"/>
+      <c r="P23" s="35"/>
       <c r="Q23" s="12"/>
       <c r="R23" s="12"/>
       <c r="S23" s="12"/>
-      <c r="T23" s="48"/>
+      <c r="T23" s="37"/>
     </row>
     <row r="24" spans="1:20">
-      <c r="A24" s="43"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="44"/>
-      <c r="J24" s="54"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="33"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
-      <c r="N24" s="53"/>
-      <c r="P24" s="43"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="44"/>
+      <c r="N24" s="42"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="33"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="A25" s="46"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="47"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="57"/>
-      <c r="N25" s="47"/>
-      <c r="P25" s="46"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="36"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="46"/>
+      <c r="N25" s="36"/>
+      <c r="P25" s="35"/>
       <c r="Q25" s="6"/>
-      <c r="R25" s="36"/>
-      <c r="S25" s="36"/>
-      <c r="T25" s="47"/>
+      <c r="R25" s="28"/>
+      <c r="S25" s="28"/>
+      <c r="T25" s="36"/>
     </row>
     <row r="26" spans="1:20">
-      <c r="A26" s="46"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="12"/>
       <c r="C26" s="7"/>
       <c r="D26" s="12"/>
-      <c r="E26" s="47"/>
-      <c r="J26" s="46"/>
+      <c r="E26" s="36"/>
+      <c r="J26" s="35"/>
       <c r="K26" s="12"/>
-      <c r="L26" s="39"/>
+      <c r="L26" s="31"/>
       <c r="M26" s="12"/>
-      <c r="N26" s="47"/>
-      <c r="P26" s="46"/>
+      <c r="N26" s="36"/>
+      <c r="P26" s="35"/>
       <c r="Q26" s="12"/>
       <c r="R26" s="7"/>
       <c r="S26" s="12"/>
-      <c r="T26" s="47"/>
+      <c r="T26" s="36"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="A27" s="46"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="47"/>
-      <c r="J27" s="46"/>
+      <c r="E27" s="36"/>
+      <c r="J27" s="35"/>
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="47"/>
-      <c r="P27" s="46"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="36"/>
+      <c r="P27" s="35"/>
       <c r="Q27" s="12"/>
       <c r="R27" s="12"/>
       <c r="S27" s="6"/>
-      <c r="T27" s="47"/>
+      <c r="T27" s="36"/>
     </row>
     <row r="28" spans="1:20" ht="15" thickBot="1">
-      <c r="A28" s="49"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="51"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="58"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="50"/>
-      <c r="S28" s="50"/>
-      <c r="T28" s="51"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="40"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="47"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="39"/>
+      <c r="S28" s="39"/>
+      <c r="T28" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="P11:S11"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="P18:T18"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="K13:N13"/>
     <mergeCell ref="K14:N14"/>
     <mergeCell ref="E9:I9"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="P11:S11"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="P18:T18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>